<commit_message>
Added format to read seconds
</commit_message>
<xml_diff>
--- a/Dataset/DS FUEL USED.xlsx
+++ b/Dataset/DS FUEL USED.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yosef\OneDrive\Escritorio\Fuel\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yosef\OneDrive\Documents\3DTracking\Fuel_Data\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36B253F-4F97-4D0D-A574-F317E3B8F939}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6797A869-CD90-4C68-A219-20F4D2979A44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="915" windowWidth="20400" windowHeight="10155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -199,6 +199,13 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,7 +523,7 @@
   <dimension ref="A1:F2658"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1"/>
@@ -524,7 +531,7 @@
     <col min="1" max="1" width="0" style="7" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="4" max="4" width="20" style="14" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
@@ -539,7 +546,7 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -53659,7 +53666,7 @@
       <c r="C2657" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2657" s="4" t="s">
+      <c r="D2657" s="13" t="s">
         <v>0</v>
       </c>
       <c r="E2657" s="4">
@@ -53679,7 +53686,7 @@
       <c r="C2658" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2658" s="4" t="s">
+      <c r="D2658" s="13" t="s">
         <v>0</v>
       </c>
       <c r="E2658" s="4">
@@ -53691,5 +53698,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>